<commit_message>
cập nhật tuần 2, 3
</commit_message>
<xml_diff>
--- a/Kế hoạch 10 tuần.xlsx
+++ b/Kế hoạch 10 tuần.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN DỰ ÁN CÔNG NGHỆ THÔNG TIN 2</t>
   </si>
@@ -114,6 +114,12 @@
     <t>Đã viết ra các bước usecase
 Xây dựng ERD 50%
 ProcessFlow chart 30%</t>
+  </si>
+  <si>
+    <t>Đã xác định các phần tử trên cisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đã có giao diện </t>
   </si>
 </sst>
 </file>
@@ -545,8 +551,8 @@
   </sheetPr>
   <dimension ref="A1:AC985"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -960,8 +966,12 @@
       <c r="D11" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="E11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="21">
+        <v>0.6</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1001,8 +1011,12 @@
       <c r="D12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="21">
+        <v>0.5</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>

</xml_diff>

<commit_message>
Cập nhật tình hình tuần 4, 5
</commit_message>
<xml_diff>
--- a/Kế hoạch 10 tuần.xlsx
+++ b/Kế hoạch 10 tuần.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN DỰ ÁN CÔNG NGHỆ THÔNG TIN 2</t>
   </si>
@@ -119,7 +119,15 @@
     <t>Đã xác định các phần tử trên cisco</t>
   </si>
   <si>
-    <t xml:space="preserve">Đã có giao diện </t>
+    <t xml:space="preserve">Đã có giao diện 
+</t>
+  </si>
+  <si>
+    <t>Xây dựng cơ bản trên Cisco
+Bổ sung ERD
+Bổ sung Flowchart
+Chỉnh sửa thiết kế chức năng
+Code database theo sơ đồ ERD</t>
   </si>
 </sst>
 </file>
@@ -551,8 +559,8 @@
   </sheetPr>
   <dimension ref="A1:AC985"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1049,7 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" spans="1:29" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="70.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>6</v>
       </c>
@@ -1056,8 +1064,12 @@
       <c r="D13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="21">
+        <v>0.5</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>

</xml_diff>